<commit_message>
change theme Python code block
</commit_message>
<xml_diff>
--- a/examples/data/multi_ink_losses_estimated_annual_losses/output/hazard_names.xlsx
+++ b/examples/data/multi_ink_losses_estimated_annual_losses/output/hazard_names.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -543,50 +543,6 @@
         </is>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>RP_1000</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>maximum</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>RP1000_ma</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>data\multi_ink_losses_estimated_annual_losses\static\hazard\RP_1000.tif</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>RP_1000</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>fraction of network segment impacted by hazard</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>RP1000_fr</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>data\multi_ink_losses_estimated_annual_losses\static\hazard\RP_1000.tif</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>